<commit_message>
added flyback diode and worked on routing
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D242002-1DFF-4A1A-950C-01EB7B23B0DA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A564943A-98FA-4FF6-9BDF-A4A8285E469B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Part</t>
   </si>
@@ -42,16 +42,28 @@
     <t>T1</t>
   </si>
   <si>
-    <t>NPN for relay</t>
-  </si>
-  <si>
     <t>Digikey Part Num</t>
   </si>
   <si>
-    <t>MMBT3904TPMSCT-ND</t>
-  </si>
-  <si>
     <t>Voltage regulator 5V@0.5A</t>
+  </si>
+  <si>
+    <t>N MOSFET for relay</t>
+  </si>
+  <si>
+    <t>NTR4003NT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>flyback diode for relay</t>
+  </si>
+  <si>
+    <t>1655-1502-1-ND</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>AZ2940D-5.0TRE1DICT-ND</t>
   </si>
 </sst>
 </file>
@@ -403,16 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617394E4-11B6-4106-A12B-6809128902C2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -423,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,15 +443,29 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
found MOSFET and transistor
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482AA9AD-745C-42E7-A1DA-E4CE63CF1DF7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7E54EA-F1D8-4226-936D-F0639E2725D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Part</t>
   </si>
@@ -45,16 +45,19 @@
     <t>Digikey Part Num</t>
   </si>
   <si>
-    <t>Voltage regulator 5V@0.5A</t>
-  </si>
-  <si>
     <t>NTR4003NT1GOSCT-ND</t>
   </si>
   <si>
-    <t>AZ2940D-5.0TRE1DICT-ND</t>
-  </si>
-  <si>
     <t>N MOSFET for e-stop</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>VSKY20301608-G4-08GICT-ND</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -409,13 +412,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -434,18 +437,21 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beginning work on the BOM
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7E54EA-F1D8-4226-936D-F0639E2725D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C8F667-3612-4C4F-85F1-6623547549BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Part</t>
   </si>
@@ -39,18 +39,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>Digikey Part Num</t>
   </si>
   <si>
     <t>NTR4003NT1GOSCT-ND</t>
   </si>
   <si>
-    <t>N MOSFET for e-stop</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -58,6 +52,15 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>T1,2</t>
+  </si>
+  <si>
+    <t>N MOSFET</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617394E4-11B6-4106-A12B-6809128902C2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,7 +424,7 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,29 +432,35 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote BOM - no connectors
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C8F667-3612-4C4F-85F1-6623547549BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D4F9A1-037E-4021-8C7C-D3A4141A30BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Part</t>
   </si>
@@ -45,9 +45,6 @@
     <t>NTR4003NT1GOSCT-ND</t>
   </si>
   <si>
-    <t>Diode</t>
-  </si>
-  <si>
     <t>VSKY20301608-G4-08GICT-ND</t>
   </si>
   <si>
@@ -61,19 +58,106 @@
   </si>
   <si>
     <t>N MOSFET</t>
+  </si>
+  <si>
+    <t>507-1773-1-ND</t>
+  </si>
+  <si>
+    <t>1.5 A fuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>From LIDAR board</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>1K 0603 Resistor</t>
+  </si>
+  <si>
+    <t>541-3991-2-ND</t>
+  </si>
+  <si>
+    <t>Spares included</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>5V REG</t>
+  </si>
+  <si>
+    <t>NCP59151DS50R4GOSCT-ND</t>
+  </si>
+  <si>
+    <t>P975-ND</t>
+  </si>
+  <si>
+    <t>10 uF Cap</t>
+  </si>
+  <si>
+    <t>401-1426-1-ND</t>
+  </si>
+  <si>
+    <t>Reset Button</t>
+  </si>
+  <si>
+    <t>490-13247-1-ND</t>
+  </si>
+  <si>
+    <t>47 uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t>BAS16HT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>Signal Diodes</t>
+  </si>
+  <si>
+    <t>Power diode</t>
+  </si>
+  <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
+    <t>Green SMD LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,8 +180,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,19 +501,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617394E4-11B6-4106-A12B-6809128902C2}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,15 +526,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -452,15 +543,130 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed up BOM and renamed test points to useful names
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D4F9A1-037E-4021-8C7C-D3A4141A30BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D5B41-6A06-4C3E-891B-6A16AF6D809E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Part</t>
   </si>
@@ -51,9 +51,6 @@
     <t>D4</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>T1,2</t>
   </si>
   <si>
@@ -78,12 +75,6 @@
     <t>1K 0603 Resistor</t>
   </si>
   <si>
-    <t>541-3991-2-ND</t>
-  </si>
-  <si>
-    <t>Spares included</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -127,12 +118,39 @@
   </si>
   <si>
     <t>Green SMD LED</t>
+  </si>
+  <si>
+    <t>Quantity on Board</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Verified pinout</t>
+  </si>
+  <si>
+    <t>541-3991-1-ND</t>
+  </si>
+  <si>
+    <t>Buying 10 is cheaper than buying 3.</t>
+  </si>
+  <si>
+    <t>Not SBAS16HT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,13 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,21 +520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617394E4-11B6-4106-A12B-6809128902C2}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,15 +548,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -542,13 +573,26 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="4">
+        <f>E2*F2</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -556,117 +600,227 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G12" si="0">E3*F3</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.88</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="4">
+        <f>SUM(G2:G12)</f>
+        <v>9.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed most of Will's critiques
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D5B41-6A06-4C3E-891B-6A16AF6D809E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722649EC-E4FB-4E2D-BE18-F0750DF49F91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Part</t>
   </si>
@@ -99,9 +98,6 @@
     <t>Reset Button</t>
   </si>
   <si>
-    <t>490-13247-1-ND</t>
-  </si>
-  <si>
     <t>47 uF Ceramic Cap</t>
   </si>
   <si>
@@ -142,6 +138,12 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>587-1780-1-ND</t>
+  </si>
+  <si>
+    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -523,7 +525,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,16 +550,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -584,7 +586,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -592,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -646,7 +648,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -665,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -732,23 +734,26 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -774,10 +779,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -793,15 +798,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -820,7 +825,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G14" s="4">
         <f>SUM(G2:G12)</f>
-        <v>9.98</v>
+        <v>10.879999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added decoupling caps to neopixles and Arduino
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722649EC-E4FB-4E2D-BE18-F0750DF49F91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3C46B-E6B6-4598-8C3C-048D437CA81C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Part</t>
   </si>
@@ -86,12 +87,6 @@
     <t>NCP59151DS50R4GOSCT-ND</t>
   </si>
   <si>
-    <t>P975-ND</t>
-  </si>
-  <si>
-    <t>10 uF Cap</t>
-  </si>
-  <si>
     <t>401-1426-1-ND</t>
   </si>
   <si>
@@ -143,7 +138,16 @@
     <t>587-1780-1-ND</t>
   </si>
   <si>
-    <t>NEW</t>
+    <t>100 uF Electrolytic Cap</t>
+  </si>
+  <si>
+    <t>1uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t>1276-1182-1-ND</t>
+  </si>
+  <si>
+    <t>732-8598-1-ND</t>
   </si>
 </sst>
 </file>
@@ -522,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617394E4-11B6-4106-A12B-6809128902C2}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,16 +554,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -586,7 +590,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -594,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -609,7 +613,7 @@
         <v>0.38</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G12" si="0">E3*F3</f>
+        <f t="shared" ref="G3:G13" si="0">E3*F3</f>
         <v>0.76</v>
       </c>
     </row>
@@ -648,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -667,7 +671,7 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -713,10 +717,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -725,43 +729,40 @@
         <v>2</v>
       </c>
       <c r="F8" s="4">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>0.54</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F9" s="4">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>2.0999999999999996</v>
-      </c>
-      <c r="H9" t="s">
-        <v>37</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
         <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -770,62 +771,83 @@
         <v>2</v>
       </c>
       <c r="F10" s="4">
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>1.04</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
       </c>
       <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G14" s="4">
-        <f>SUM(G2:G12)</f>
-        <v>10.879999999999999</v>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="4">
+        <f>SUM(G2:G13)</f>
+        <v>10.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Control board ready to order
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3C46B-E6B6-4598-8C3C-048D437CA81C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEB4220-187A-4AAF-BD07-0A0FDBB2475D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>541-3991-1-ND</t>
   </si>
   <si>
-    <t>Buying 10 is cheaper than buying 3.</t>
-  </si>
-  <si>
     <t>Not SBAS16HT1GOSCT-ND</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>732-8598-1-ND</t>
+  </si>
+  <si>
+    <t>Buying 10 is cheaper than buying 4.</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +563,7 @@
         <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -671,7 +671,7 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -717,10 +717,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -738,23 +738,23 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="4">
         <v>0.1</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -820,7 +820,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -847,7 +847,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G15" s="4">
         <f>SUM(G2:G13)</f>
-        <v>10.34</v>
+        <v>10.440000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exported CAM files and added labeling to schematic
</commit_message>
<xml_diff>
--- a/sedani/chassis_control_board/control_board_3.1_parts.xlsx
+++ b/sedani/chassis_control_board/control_board_3.1_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Robojackets\roboracing-electrical\sedani\chassis_control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEB4220-187A-4AAF-BD07-0A0FDBB2475D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E681CE-E9DD-4108-B669-2F5F5618A51B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{7A34FA13-F12C-431D-B67E-F7A4D3A95559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>